<commit_message>
Corrected BOM and added price calculation
</commit_message>
<xml_diff>
--- a/Rev. 1/Excel/C64_PSU_Global_BoM_v1_0.xlsx
+++ b/Rev. 1/Excel/C64_PSU_Global_BoM_v1_0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projekte\_Eigene\C64-Projects\C64 PSU GLOBAL\Rev. 1\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9239083C-BC0B-4700-8CD8-077FE4D6C773}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780CA5B5-8D82-4996-A824-6918EBC3C584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5712" yWindow="2964" windowWidth="21012" windowHeight="13728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34644" yWindow="2532" windowWidth="21012" windowHeight="13728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
@@ -241,9 +241,6 @@
     <t>2x2p, 2.54mm</t>
   </si>
   <si>
-    <t>2x3p, 2.54mm</t>
-  </si>
-  <si>
     <t>09503021</t>
   </si>
   <si>
@@ -848,6 +845,9 @@
   </si>
   <si>
     <t>countersunk screw for sheet metal or plastic</t>
+  </si>
+  <si>
+    <t>2x4p, 2.54mm</t>
   </si>
 </sst>
 </file>
@@ -1975,8 +1975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F162"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1991,7 +1991,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -2001,7 +2001,7 @@
     </row>
     <row r="2" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -2067,7 +2067,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -2079,14 +2079,14 @@
         <v>1</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -2098,14 +2098,14 @@
         <v>3</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2159,14 +2159,14 @@
         <v>1</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="5" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2178,14 +2178,14 @@
         <v>2</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2197,14 +2197,14 @@
         <v>1</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2213,7 +2213,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>68</v>
@@ -2237,7 +2237,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>18</v>
@@ -2258,14 +2258,14 @@
         <v>5</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2286,7 +2286,7 @@
         <v>21</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2298,14 +2298,14 @@
         <v>1</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="5" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
@@ -2317,14 +2317,14 @@
         <v>2</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2345,7 +2345,7 @@
         <v>23</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2357,14 +2357,14 @@
         <v>1</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2376,14 +2376,14 @@
         <v>4</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2404,7 +2404,7 @@
         <v>25</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2416,14 +2416,14 @@
         <v>1</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2435,14 +2435,14 @@
         <v>3</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2454,7 +2454,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25" s="13">
         <v>318211</v>
@@ -2463,7 +2463,7 @@
         <v>26</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2475,14 +2475,14 @@
         <v>1</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2494,14 +2494,14 @@
         <v>1</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2522,7 +2522,7 @@
         <v>29</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2534,7 +2534,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>30</v>
@@ -2543,7 +2543,7 @@
         <v>31</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="5" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
@@ -2555,14 +2555,14 @@
         <v>1</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="5" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
@@ -2574,14 +2574,14 @@
         <v>4</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D31" s="13"/>
       <c r="E31" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2593,14 +2593,14 @@
         <v>1</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -2621,7 +2621,7 @@
         <v>34</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2642,7 +2642,7 @@
         <v>37</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -2663,7 +2663,7 @@
         <v>40</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2684,7 +2684,7 @@
         <v>43</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="5" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
@@ -2705,7 +2705,7 @@
         <v>45</v>
       </c>
       <c r="F37" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -2726,7 +2726,7 @@
         <v>48</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2738,7 +2738,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>49</v>
@@ -2747,7 +2747,7 @@
         <v>50</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="5" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
@@ -2768,7 +2768,7 @@
         <v>53</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -2789,7 +2789,7 @@
         <v>56</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="5" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
@@ -2810,7 +2810,7 @@
         <v>59</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -2831,7 +2831,7 @@
         <v>62</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2843,12 +2843,12 @@
         <v>1</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="5" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
@@ -2860,12 +2860,12 @@
         <v>1</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D45" s="17"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="5" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
@@ -2874,15 +2874,15 @@
         <v>43</v>
       </c>
       <c r="B46" s="12">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D46" s="17"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2894,12 +2894,12 @@
         <v>1</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2908,15 +2908,15 @@
         <v>45</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D48" s="17"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2928,12 +2928,12 @@
         <v>4</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D49" s="17"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2945,12 +2945,12 @@
         <v>1</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D50" s="13"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2962,14 +2962,14 @@
         <v>1</v>
       </c>
       <c r="C51" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D51" s="13" t="s">
         <v>145</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>146</v>
       </c>
       <c r="E51" s="12"/>
       <c r="F51" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2981,12 +2981,12 @@
         <v>1</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D52" s="13"/>
       <c r="E52" s="12"/>
       <c r="F52" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -2995,15 +2995,15 @@
         <v>50</v>
       </c>
       <c r="B53" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C53" s="12" t="s">
         <v>151</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>152</v>
       </c>
       <c r="D53" s="13"/>
       <c r="E53" s="12"/>
       <c r="F53" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3012,15 +3012,15 @@
         <v>51</v>
       </c>
       <c r="B54" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C54" s="12" t="s">
         <v>155</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>156</v>
       </c>
       <c r="D54" s="13"/>
       <c r="E54" s="12"/>
       <c r="F54" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3029,15 +3029,15 @@
         <v>52</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D55" s="13"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="5" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
@@ -3046,10 +3046,10 @@
         <v>53</v>
       </c>
       <c r="B56" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C56" s="12" t="s">
         <v>159</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>160</v>
       </c>
       <c r="D56" s="13"/>
       <c r="E56" s="12"/>
@@ -3061,10 +3061,10 @@
         <v>54</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D57" s="13"/>
       <c r="E57" s="12"/>
@@ -3079,12 +3079,12 @@
         <v>1</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D58" s="13"/>
       <c r="E58" s="12"/>
       <c r="F58" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3096,12 +3096,12 @@
         <v>4</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D59" s="13"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3113,12 +3113,12 @@
         <v>8</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D60" s="13"/>
       <c r="E60" s="12"/>
       <c r="F60" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3130,12 +3130,12 @@
         <v>4</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D61" s="13"/>
       <c r="E61" s="12"/>
       <c r="F61" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3147,12 +3147,12 @@
         <v>2</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D62" s="13"/>
       <c r="E62" s="12"/>
       <c r="F62" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -3164,12 +3164,12 @@
         <v>4</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D63" s="13"/>
       <c r="E63" s="12"/>
       <c r="F63" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>